<commit_message>
add more yellow data
</commit_message>
<xml_diff>
--- a/Data/Filters.xlsx
+++ b/Data/Filters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/pf522_ic_ac_uk/Documents/lab3/Photoelectric/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="350" documentId="8_{B11BF44A-BC13-47B3-A806-A4FE40F6A6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22A8B053-9964-4438-9CB7-37036C49A702}"/>
+  <xr:revisionPtr revIDLastSave="368" documentId="8_{B11BF44A-BC13-47B3-A806-A4FE40F6A6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADFE5122-626B-4B8A-B975-9DE50EF608D6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{07B0476E-BC55-49DF-8EAE-3E97C97846C3}"/>
   </bookViews>
@@ -1392,7 +1392,7 @@
                   <c:v>16650</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>18332</c:v>
+                  <c:v>23432</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
                   <c:v>58445</c:v>
@@ -1841,8 +1841,26 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
+                <c:pt idx="10" formatCode="0.00E+00">
+                  <c:v>-1.361</c:v>
+                </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
                   <c:v>-3.08</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.7190000000000003</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="0.00E+00">
+                  <c:v>59.1</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="0.00E+00">
+                  <c:v>140.9</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="0.00E+00">
+                  <c:v>1403</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="0.00E+00">
+                  <c:v>3494</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
                   <c:v>8001</c:v>
@@ -4748,7 +4766,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y27" sqref="Y27:Z27"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4980,6 +4998,12 @@
       <c r="G12" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
+      <c r="H12" s="1">
+        <v>-1.361</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.115</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -5104,6 +5128,12 @@
       <c r="E20" s="1">
         <v>0.34399999999999997</v>
       </c>
+      <c r="H20">
+        <v>6.7190000000000003</v>
+      </c>
+      <c r="I20">
+        <v>7.6600000000000001E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -5115,6 +5145,12 @@
       <c r="E21" s="1">
         <v>1.905</v>
       </c>
+      <c r="H21" s="1">
+        <v>59.1</v>
+      </c>
+      <c r="I21">
+        <v>1.9059999999999999</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -5138,6 +5174,12 @@
       <c r="G22" s="1">
         <v>412</v>
       </c>
+      <c r="H22" s="1">
+        <v>140.9</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0.94399999999999995</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -5161,6 +5203,12 @@
       <c r="G23" s="1">
         <v>168.2</v>
       </c>
+      <c r="H23" s="1">
+        <v>1403</v>
+      </c>
+      <c r="I23" s="1">
+        <v>57.9</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -5184,6 +5232,12 @@
       <c r="G24" s="1">
         <v>46.4</v>
       </c>
+      <c r="H24" s="1">
+        <v>3494</v>
+      </c>
+      <c r="I24" s="1">
+        <v>196</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -5202,7 +5256,7 @@
         <v>1287</v>
       </c>
       <c r="F25" s="1">
-        <v>18332</v>
+        <v>23432</v>
       </c>
       <c r="G25" s="1">
         <v>359</v>

</xml_diff>